<commit_message>
Fork from https://github.com/Mokwang/Minnow3build and update.
1. Fork from https://github.com/Mokwang/Minnow3build to backup
2. Update excel for latest test scope.
3. Remove password for svn link

Signed-off-by: wangbinx <binx.a.wang@intel.com>
</commit_message>
<xml_diff>
--- a/Readme/controller_ubuntu.xlsx
+++ b/Readme/controller_ubuntu.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>X64</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,12 +34,6 @@
     <t>FAB A</t>
   </si>
   <si>
-    <t>FAB B</t>
-  </si>
-  <si>
-    <t>Minnow3</t>
-  </si>
-  <si>
     <t>Platform</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Aurora Glacier</t>
   </si>
 </sst>
 </file>
@@ -129,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,24 +143,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,9 +162,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -485,9 +460,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -500,13 +477,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -516,82 +493,48 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>4</v>
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1"/>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+    <row r="4" spans="1:5" ht="29.25" customHeight="1"/>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Add new type of build and remove Minnow3.
Add Disable_flash_region_access(R) type to build type list.
Remove Minnowboard3
Change share path
</commit_message>
<xml_diff>
--- a/Readme/controller_ubuntu.xlsx
+++ b/Readme/controller_ubuntu.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>X64</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,19 +49,10 @@
     <t>"Y" is build this image and "N/A" is not build the image</t>
   </si>
   <si>
-    <t>Minnow3 Module</t>
-  </si>
-  <si>
     <t>Leaf Hill</t>
   </si>
   <si>
     <t>FAB D</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>FAB C</t>
   </si>
   <si>
     <t>UP2</t>
@@ -100,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,12 +107,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEBFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,9 +159,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -503,7 +485,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -517,10 +499,10 @@
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -532,49 +514,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1"/>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
+    <row r="4" spans="1:5" ht="29.25" customHeight="1"/>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>